<commit_message>
Every thing is working fine
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -2261,7 +2261,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Alt attribute present: Quédate en el corazón de Porto</t>
+          <t>Alt attribute present: Gran oferta para esta noche</t>
         </is>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Alt attribute present: Villa de lujo a partir de Hotala™ 55</t>
+          <t>Alt attribute present: Reservado 7 veces en las últimas 24 horas</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Alt attribute present: Reserva de última hora en Porto</t>
+          <t>Alt attribute present: Casa mejor calificada en Porto</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Alt attribute present: Casa de estilo único en Porto</t>
+          <t>Alt attribute present: Casa excepcional cerca de Porto</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Alt attribute present: Tarifas calientes hoy.  Porto Descuentos</t>
+          <t>Alt attribute present: Alquiler de viviendas de lujo a Hotala™ 99</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Alt attribute present: Alquiler de viviendas de lujo a Hotala™ 99</t>
+          <t>Alt attribute present: Casa ecológica en Porto</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/modern-apartment-with-balcony-and-free-parking/BC-11172109</t>
+          <t>https://www.alojamiento.io/all/andorra</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/catalonia</t>
+          <t>https://www.alojamiento.io/all/greece</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2823,7 +2823,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/canary-islands/gran-canaria</t>
+          <t>https://www.alojamiento.io/near-me?all=true</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/guatemala/sacatepequez/antigua-guatemala</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/hotels</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2873,7 +2873,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/quintana-roo/tulum</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2134335&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=2-BC-2134335&amp;published=true&amp;dest_id=2134335&amp;hero=BC-1935047&amp;owner_id=2134335&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-09-04T08%3A44%3A02.076302%2B00%3A00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2898,7 +2898,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11242224&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=8-BC-11242224&amp;published=true&amp;dest_id=11242224&amp;hero=BC-1935047&amp;owner_id=11242224&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T17%3A21%3A13.957523%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/argentina/mendoza</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2923,7 +2923,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/dominican-republic/la-altagracia/punta-cana</t>
+          <t>https://www.alojamiento.io/property/romantic-luxury-house-w-captivating-outdoor-patio/BC-10659330</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/near-me?all=true</t>
+          <t>https://www.alojamiento.io/all/honduras/bay-islands/roatan</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2973,7 +2973,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/site-terms</t>
+          <t>https://www.alojamiento.io/about-us</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2998,7 +2998,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2134335&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=2-BC-2134335&amp;published=true&amp;dest_id=2134335&amp;hero=BC-1935047&amp;owner_id=2134335&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-09-04T08%3A44%3A02.076302%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/catalonia/costa-brava</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3023,7 +3023,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/galicia</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166825172&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=9-HA-6166825172&amp;published=true&amp;dest_id=18971561&amp;hero=BC-1935047&amp;owner_id=18971561&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A03%3A04.951386%2B00%3A00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3048,7 +3048,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/canary-islands/tenerife</t>
+          <t>https://www.alojamiento.io/all/mexico/quintana-roo/cancun</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3073,7 +3073,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/argentina/buenos-aires</t>
+          <t>https://www.alojamiento.io/all/spain/community-of-madrid/madrid</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/resorts</t>
+          <t>https://www.alojamiento.io/all/spain/catalonia</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3123,7 +3123,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847410&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=23-BC-12847410&amp;published=true&amp;dest_id=12847410&amp;hero=BC-1935047&amp;owner_id=12847410&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A18%3A47.203235%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/italy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3148,7 +3148,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/peru/lima</t>
+          <t>https://www.alojamiento.io/site-map</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -3173,7 +3173,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/romantic-luxury-house-w-captivating-outdoor-patio/BC-10659330</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=4-placeholder5&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3198,7 +3198,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/vila-cam%c3%a9lia/BC-11099494</t>
+          <t>https://www.alojamiento.io/property/cozy-apartment-invicta-city-opo/BC-11534173</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3223,7 +3223,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11105844&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=22-BC-11105844&amp;published=true&amp;dest_id=11105844&amp;hero=BC-1935047&amp;owner_id=11105844&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T11%3A25%3A32.784787%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/panama/panama/panama-city</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/casa-velha-guesthouse/BC-2782646</t>
+          <t>https://www.alojamiento.io/privacy-policy#site-cookie-policy</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3273,7 +3273,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/cuba/province-of-havana</t>
+          <t>https://www.alojamiento.io/all/guatemala/sacatepequez/antigua-guatemala</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/quintana-roo/playa-del-carmen</t>
+          <t>https://www.alojamiento.io/place-to-stay</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3323,7 +3323,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/quintana-roo/cancun</t>
+          <t>https://www.alojamiento.io/property/urban-views-bright-apt-inspired-by-pal%c3%a1cio-cristal/HA-61611682440</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3348,7 +3348,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/argentina/rio-negro/san-carlos-de-bariloche</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11172109&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=13-BC-11172109&amp;published=true&amp;dest_id=11172109&amp;hero=BC-1935047&amp;owner_id=11172109&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T15%3A02%3A53.704870%2B00%3A00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3373,7 +3373,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/navarre</t>
+          <t>https://www.alojamiento.io/all/cuba/province-of-havana</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/ecuador/pichincha/quito</t>
+          <t>https://www.alojamiento.io/addalisting</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3423,7 +3423,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2782646&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=18-BC-2782646&amp;published=true&amp;dest_id=2782646&amp;hero=BC-1935047&amp;owner_id=2782646&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-06T15%3A45%3A49.219738%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11534173&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=10-BC-11534173&amp;published=true&amp;dest_id=11534173&amp;hero=BC-1935047&amp;owner_id=11534173&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-05-12T13%3A17%3A41.359928%2B00%3A00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3448,7 +3448,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166825172&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=9-HA-6166825172&amp;published=true&amp;dest_id=18971561&amp;hero=BC-1935047&amp;owner_id=18971561&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A03%3A04.951386%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/argentina/buenos-aires</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3473,7 +3473,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10659330&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=12-BC-10659330&amp;published=true&amp;dest_id=10659330&amp;hero=BC-1935047&amp;owner_id=10659330&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T06%3A05%3A00.026562%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/campo-lindo-apartment/BC-1935047</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3498,7 +3498,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/colombia/medellin</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10998286&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=11-BC-10998286&amp;published=true&amp;dest_id=10998286&amp;hero=BC-1935047&amp;owner_id=10998286&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T07%3A15%3A38.030190%2B00%3A00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3523,7 +3523,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/cozy-apartment-invicta-city-opo/BC-11534173</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10599206&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=14-BC-10599206&amp;published=true&amp;dest_id=10599206&amp;hero=BC-1935047&amp;owner_id=10599206&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-16T03%3A31%3A23.472631%2B00%3A00</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/about-us</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=2-placeholder3&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3573,7 +3573,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/villas</t>
+          <t>https://x.com/StaysTravel</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -3591,14 +3591,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/ac-house/BC-2807903</t>
+          <t>https://www.alojamiento.io/all/mexico</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3623,7 +3623,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/lux-in-porto/BC-10998286</t>
+          <t>https://www.alojamiento.io/refine?search=Paranhos%2c%20Porto%2c%20Porto%20District%2c%20Portugal</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3648,7 +3648,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/brazil/south-region/florianopolis</t>
+          <t>https://www.alojamiento.io/all/mexico/guanajuato/san-miguel-de-allende</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3673,7 +3673,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.travelai.com/</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11099494&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=17-BC-11099494&amp;published=true&amp;dest_id=11099494&amp;hero=BC-1935047&amp;owner_id=11099494&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-01T07%3A14%3A52.613135%2B00%3A00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3691,14 +3691,14 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Status code 200 (OK)</t>
+          <t>Status code 403 (Forbidden)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto</t>
+          <t>https://www.alojamiento.io/all/brazil/south-region/florianopolis</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3723,7 +3723,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/renovado-com-ac-2-wc-completos-terra%c3%a7o-e-garagem/BC-12500411</t>
+          <t>https://www.alojamiento.io/property/vila-cam%c3%a9lia/BC-11099494</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3748,7 +3748,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/colombia/bolivar/cartagena</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6118850658&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=5-HA-6118850658&amp;published=true&amp;dest_id=29545296&amp;hero=BC-1935047&amp;owner_id=29545296&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T11%3A48%3A37.454906%2B00%3A00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3773,7 +3773,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/lovely-flat-marqu%c3%aas/BC-11105844</t>
+          <t>https://www.alojamiento.io/all/costa-rica/san-jose</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3798,7 +3798,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-31/BC-12847410</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11242224&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=8-BC-11242224&amp;published=true&amp;dest_id=11242224&amp;hero=BC-1935047&amp;owner_id=11242224&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T17%3A21%3A13.957523%2B00%3A00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3823,7 +3823,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=3-placeholder4&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4649516&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=19-BC-4649516&amp;published=true&amp;dest_id=4649516&amp;hero=BC-1935047&amp;owner_id=4649516&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-08-24T10%3A49%3A52.209651%2B00%3A00</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/andorra</t>
+          <t>https://www.alojamiento.io/property/modern-apartment-with-balcony-and-free-parking/BC-11172109</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3873,7 +3873,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.onedegreeleft.com/</t>
+          <t>https://www.alojamiento.io/all/morocco</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -3891,14 +3891,14 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Status code 200 (OK)</t>
+          <t>Status code 403 (Forbidden)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico</t>
+          <t>https://www.alojamiento.io/all/belize/belize-district/belize-city</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3948,7 +3948,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district</t>
+          <t>https://www.travelai.com/</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3957,7 +3957,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -3966,14 +3966,14 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=2-placeholder3&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/resorts</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10998286&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=11-BC-10998286&amp;published=true&amp;dest_id=10998286&amp;hero=BC-1935047&amp;owner_id=10998286&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T07%3A15%3A38.030190%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/colombia/medellin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4023,7 +4023,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/guanajuato/san-miguel-de-allende</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847410&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=23-BC-12847410&amp;published=true&amp;dest_id=12847410&amp;hero=BC-1935047&amp;owner_id=12847410&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A18%3A47.203235%2B00%3A00</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4048,7 +4048,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/faq</t>
+          <t>https://www.alojamiento.io/property/poetikblue-by-we-do-living/BC-11346246</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4073,7 +4073,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11099494&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=17-BC-11099494&amp;published=true&amp;dest_id=11099494&amp;hero=BC-1935047&amp;owner_id=11099494&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-01T07%3A14%3A52.613135%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=1-placeholder2&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4098,7 +4098,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/quarto-duplo-com-casa-de-banho-exclusiva-no-porto/BC-10599206</t>
+          <t>https://www.alojamiento.io/all/mexico/baja-california-sur/cabo-san-lucas</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4123,7 +4123,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/jalisco/puerto-vallarta</t>
+          <t>https://www.alojamiento.io/all/spain/canary-islands</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/usa/wyoming/basin</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847446&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=15-BC-12847446&amp;published=true&amp;dest_id=12847446&amp;hero=BC-1935047&amp;owner_id=12847446&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A19%3A35.025518%2B00%3A00</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4173,7 +4173,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/cantabria</t>
+          <t>https://www.alojamiento.io/property/s-jo%c3%a3o-porto-apartment/BC-2202420</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4198,7 +4198,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682438&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=3-HA-61611682438&amp;published=true&amp;dest_id=109825542&amp;hero=BC-1935047&amp;owner_id=109825542&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373667%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/navarre</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4223,7 +4223,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/greece</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=5-placeholder6&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4248,7 +4248,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=1-placeholder2&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/spain/castile-and-leon</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4273,7 +4273,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2202420&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=4-BC-2202420&amp;published=true&amp;dest_id=2202420&amp;hero=BC-1935047&amp;owner_id=2202420&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-12-06T11%3A00%3A04.420388%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/mexico/jalisco/puerto-vallarta</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/panama/panama/panama-city</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/villas</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4323,7 +4323,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/chile/santiago-metropolitan/santiago</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11105844&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=22-BC-11105844&amp;published=true&amp;dest_id=11105844&amp;hero=BC-1935047&amp;owner_id=11105844&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T11%3A25%3A32.784787%2B00%3A00</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -4348,7 +4348,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/uruguay/montevideo</t>
+          <t>https://www.alojamiento.io/all/france</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -4373,7 +4373,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11346246&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=21-BC-11346246&amp;published=true&amp;dest_id=11346246&amp;hero=BC-1935047&amp;owner_id=11346246&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-09-22T08%3A32%3A12.548999%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/colombia/magdalena/santa-marta</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -4398,7 +4398,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/portogali-guesthouse/BC-5813166</t>
+          <t>https://www.alojamiento.io/property/ac-house/BC-2807903</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -4423,7 +4423,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-32/BC-12847446</t>
+          <t>https://www.alojamiento.io/all/usa/wyoming/basin</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/addalisting</t>
+          <t>https://www.alojamiento.io/all/brazil/southeast-region/rio-de-janeiro</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -4473,7 +4473,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11534173&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=10-BC-11534173&amp;published=true&amp;dest_id=11534173&amp;hero=BC-1935047&amp;owner_id=11534173&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-05-12T13%3A17%3A41.359928%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/lv-premier-marques-mq2-balc%c3%b3n-aire-acondicionado-vistas/HA-6118850658</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -4498,7 +4498,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/t1-apartamento-moderno-luz-tranquila-y-confortable-con-garaje-privado/HA-6166491756</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682438&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=3-HA-61611682438&amp;published=true&amp;dest_id=109825542&amp;hero=BC-1935047&amp;owner_id=109825542&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373667%2B00%3A00</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -4523,7 +4523,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5813166&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=6-BC-5813166&amp;published=true&amp;dest_id=5813166&amp;hero=BC-1935047&amp;owner_id=5813166&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-08-16T12%3A45%3A47.750380%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/peru/cusco/cusco</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -4548,7 +4548,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6118850658&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=5-HA-6118850658&amp;published=true&amp;dest_id=29545296&amp;hero=BC-1935047&amp;owner_id=29545296&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T11%3A48%3A37.454906%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/portogali-guesthouse/BC-5813166</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -4573,7 +4573,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cottages</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12500411&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=20-BC-12500411&amp;published=true&amp;dest_id=12500411&amp;hero=BC-1935047&amp;owner_id=12500411&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T11%3A00%3A14.620270%2B00%3A00</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/campo-lindo-apartment/BC-1935047</t>
+          <t>https://www.instagram.com/staystravel</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -4607,7 +4607,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -4616,14 +4616,14 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/community-of-madrid/madrid</t>
+          <t>https://www.alojamiento.io/site-terms</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -4648,7 +4648,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/brazil/northeast-region/salvador</t>
+          <t>https://www.alojamiento.io/all/chile/santiago-metropolitan/santiago</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -4673,7 +4673,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2807903&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=16-BC-2807903&amp;published=true&amp;dest_id=2807903&amp;hero=BC-1935047&amp;owner_id=2807903&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-11-19T09%3A57%3A24.866726%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/portugal</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -4723,7 +4723,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/colombia/magdalena/santa-marta</t>
+          <t>https://www.alojamiento.io/all/ecuador/pichincha/quito</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -4748,7 +4748,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/belize/belize-district/belize-city</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166491756&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=7-HA-6166491756&amp;published=true&amp;dest_id=18976742&amp;hero=BC-1935047&amp;owner_id=18976742&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A04%3A28.809814%2B00%3A00</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -4773,7 +4773,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/switzerland</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cottages</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -4798,7 +4798,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=4-placeholder5&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/spain/andalusia</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -4823,7 +4823,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/urban-views-petfrien-ap-inspired-by-torre-cl%c3%a9rigos/HA-61611682438</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cabins</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -4848,7 +4848,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -4873,7 +4873,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/baja-california-sur/cabo-san-lucas</t>
+          <t>https://www.alojamiento.io/property/rendez-vous-porto-ii-t1/HA-6166825172</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4898,7 +4898,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/poetikblue-by-we-do-living/BC-11346246</t>
+          <t>https://www.alojamiento.io/property/jm-alojamento-local-no-porto/BC-11242224</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4923,7 +4923,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/rendez-vous-porto-ii-t1/HA-6166825172</t>
+          <t>https://www.alojamiento.io/all/argentina/rio-negro/san-carlos-de-bariloche</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -4948,7 +4948,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-1935047&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=0-BC-1935047&amp;published=true&amp;dest_id=1935047&amp;hero=BC-1935047&amp;owner_id=1935047&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-11-19T06%3A10%3A57.061047%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/valencian-community/valencia-province</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -4973,7 +4973,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11172109&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=13-BC-11172109&amp;published=true&amp;dest_id=11172109&amp;hero=BC-1935047&amp;owner_id=11172109&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T15%3A02%3A53.704870%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/ecuador/galapagos</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -4998,7 +4998,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/france</t>
+          <t>https://www.onedegreeleft.com/</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -5007,7 +5007,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -5016,14 +5016,14 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/place-to-stay</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682440&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=1-HA-61611682440&amp;published=true&amp;dest_id=109825564&amp;hero=BC-1935047&amp;owner_id=109825564&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373975%2B00%3A00</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/site-map</t>
+          <t>https://www.alojamiento.io/all/peru/lima</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -5073,7 +5073,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.petfriendly.io/</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=0-placeholder1&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -5098,7 +5098,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos</t>
+          <t>https://www.facebook.com/StaysTravel</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -5107,7 +5107,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -5116,14 +5116,14 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cabins</t>
+          <t>https://www.alojamiento.io/faq</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -5148,7 +5148,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12500411&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=20-BC-12500411&amp;published=true&amp;dest_id=12500411&amp;hero=BC-1935047&amp;owner_id=12500411&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T11%3A00%3A14.620270%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-31/BC-12847410</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -5173,7 +5173,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/brazil/southeast-region/rio-de-janeiro</t>
+          <t>https://www.alojamiento.io/all/switzerland</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -5198,7 +5198,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/peru/cusco/cusco</t>
+          <t>https://www.alojamiento.io/property/quarto-duplo-com-casa-de-banho-exclusiva-no-porto/BC-10599206</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -5223,7 +5223,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/honduras/bay-islands/roatan</t>
+          <t>https://www.alojamiento.io/all/spain/murcia</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -5248,7 +5248,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal</t>
+          <t>https://www.alojamiento.io/property/t1-apartamento-moderno-luz-tranquila-y-confortable-con-garaje-privado/HA-6166491756</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -5273,7 +5273,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/StaysTravel</t>
+          <t>https://www.alojamiento.io/all/dominican-republic/la-altagracia/punta-cana</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -5282,7 +5282,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -5291,14 +5291,14 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Status code 200 (OK)</t>
+          <t>Status code 403 (Forbidden)</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/italy</t>
+          <t>https://www.petfriendly.io/</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -5323,7 +5323,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/argentina/mendoza</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -5348,7 +5348,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=5-placeholder6&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/spain/balearic-islands</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -5373,7 +5373,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/staystravel</t>
+          <t>https://www.alojamiento.io/all/spain/cantabria</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -5382,7 +5382,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -5391,14 +5391,14 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Status code 200 (OK)</t>
+          <t>Status code 403 (Forbidden)</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/jm-alojamento-local-no-porto/BC-11242224</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10659330&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=12-BC-10659330&amp;published=true&amp;dest_id=10659330&amp;hero=BC-1935047&amp;owner_id=10659330&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T06%3A05%3A00.026562%2B00%3A00</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -5423,7 +5423,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/hotels</t>
+          <t>https://www.alojamiento.io/property/casa-s%c3%a3o-dinis/BC-2134335</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -5448,7 +5448,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/valencian-community/valencia-province</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11346246&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=21-BC-11346246&amp;published=true&amp;dest_id=11346246&amp;hero=BC-1935047&amp;owner_id=11346246&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-09-22T08%3A32%3A12.548999%2B00%3A00</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -5473,7 +5473,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/andalusia</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-1935047&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=0-BC-1935047&amp;published=true&amp;dest_id=1935047&amp;hero=BC-1935047&amp;owner_id=1935047&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-11-19T06%3A10%3A57.061047%2B00%3A00</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -5498,7 +5498,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/privacy-policy#site-cookie-policy</t>
+          <t>https://www.alojamiento.io/all/spain/galicia</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -5523,7 +5523,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/ecuador/galapagos</t>
+          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-32/BC-12847446</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -5548,7 +5548,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/puerto-rico/san-juan</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2782646&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=18-BC-2782646&amp;published=true&amp;dest_id=2782646&amp;hero=BC-1935047&amp;owner_id=2782646&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-06T15%3A45%3A49.219738%2B00%3A00</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -5573,7 +5573,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=0-placeholder1&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/colombia/bolivar/cartagena</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -5598,7 +5598,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/casa-s%c3%a3o-dinis/BC-2134335</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=3-placeholder4&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -5623,7 +5623,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4649516&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=19-BC-4649516&amp;published=true&amp;dest_id=4649516&amp;hero=BC-1935047&amp;owner_id=4649516&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-08-24T10%3A49%3A52.209651%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/canary-islands/gran-canaria</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -5648,7 +5648,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10599206&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=14-BC-10599206&amp;published=true&amp;dest_id=10599206&amp;hero=BC-1935047&amp;owner_id=10599206&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-16T03%3A31%3A23.472631%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/fred-s-house-asprela/BC-4649516</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -5673,7 +5673,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/fred-s-house-asprela/BC-4649516</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/ski-chalets</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -5698,7 +5698,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/refine?search=Paranhos%2c%20Porto%2c%20Porto%20District%2c%20Portugal</t>
+          <t>https://www.alojamiento.io/privacy-policy</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/andalusia/malaga</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -5748,7 +5748,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>https://x.com/StaysTravel</t>
+          <t>https://www.alojamiento.io/property/lovely-flat-marqu%c3%aas/BC-11105844</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -5757,7 +5757,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -5766,14 +5766,14 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Status code 200 (OK)</t>
+          <t>Status code 403 (Forbidden)</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682440&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=1-HA-61611682440&amp;published=true&amp;dest_id=109825564&amp;hero=BC-1935047&amp;owner_id=109825564&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373975%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/uruguay/montevideo</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -5798,7 +5798,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/catalonia/costa-brava</t>
+          <t>https://www.alojamiento.io/all/brazil/northeast-region/salvador</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/privacy-policy</t>
+          <t>https://www.alojamiento.io/all/mexico/quintana-roo/tulum</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -5848,7 +5848,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/ski-chalets</t>
+          <t>https://www.alojamiento.io/all/spain/canary-islands/tenerife</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -5873,7 +5873,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/lv-premier-marques-mq2-balc%c3%b3n-aire-acondicionado-vistas/HA-6118850658</t>
+          <t>https://www.alojamiento.io/all/mexico/quintana-roo/playa-del-carmen</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -5898,7 +5898,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/castile-and-leon</t>
+          <t>https://www.alojamiento.io/property/urban-views-petfrien-ap-inspired-by-torre-cl%c3%a9rigos/HA-61611682438</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -5923,7 +5923,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/urban-views-bright-apt-inspired-by-pal%c3%a1cio-cristal/HA-61611682440</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5813166&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=6-BC-5813166&amp;published=true&amp;dest_id=5813166&amp;hero=BC-1935047&amp;owner_id=5813166&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-08-16T12%3A45%3A47.750380%2B00%3A00</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -5948,7 +5948,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847446&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=15-BC-12847446&amp;published=true&amp;dest_id=12847446&amp;hero=BC-1935047&amp;owner_id=12847446&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A19%3A35.025518%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/casa-velha-guesthouse/BC-2782646</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -5973,7 +5973,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/costa-rica/san-jose</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2202420&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=4-BC-2202420&amp;published=true&amp;dest_id=2202420&amp;hero=BC-1935047&amp;owner_id=2202420&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-12-06T11%3A00%3A04.420388%2B00%3A00</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -5998,7 +5998,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/balearic-islands</t>
+          <t>https://www.alojamiento.io/all/puerto-rico/san-juan</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -6023,7 +6023,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/murcia</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2807903&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=16-BC-2807903&amp;published=true&amp;dest_id=2807903&amp;hero=BC-1935047&amp;owner_id=2807903&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-11-19T09%3A57%3A24.866726%2B00%3A00</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -6048,7 +6048,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/canary-islands</t>
+          <t>https://www.alojamiento.io/all/spain/andalusia/malaga</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -6073,7 +6073,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/morocco</t>
+          <t>https://www.alojamiento.io/property/lux-in-porto/BC-10998286</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -6098,7 +6098,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/s-jo%c3%a3o-porto-apartment/BC-2202420</t>
+          <t>https://www.alojamiento.io/property/renovado-com-ac-2-wc-completos-terra%c3%a7o-e-garagem/BC-12500411</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -6123,7 +6123,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166491756&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733845825803&amp;referral_id=7-HA-6166491756&amp;published=true&amp;dest_id=18976742&amp;hero=BC-1935047&amp;owner_id=18976742&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A04%3A28.809814%2B00%3A00</t>
+          <t>https://www.alojamiento.io/</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">

</xml_diff>

<commit_message>
currency test printing sequence updated
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -2261,7 +2261,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Alt attribute present: Gran oferta para esta noche</t>
+          <t>Alt attribute present: Reservado 7 veces en las últimas 24 horas</t>
         </is>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Alt attribute present: Reservado 7 veces en las últimas 24 horas</t>
+          <t>Alt attribute present: Tarifas calientes hoy.  Porto Descuentos</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Alt attribute present: Casa mejor calificada en Porto</t>
+          <t>Alt attribute present: Alquiler de viviendas de lujo a Hotala™ 99</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Alt attribute present: Casa excepcional cerca de Porto</t>
+          <t>Alt attribute present: Casa ecológica en Porto</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Alt attribute present: Alquiler de viviendas de lujo a Hotala™ 99</t>
+          <t>Alt attribute present: Cabaña de estilo romántico</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Alt attribute present: Casa ecológica en Porto</t>
+          <t>Alt attribute present: Quédate en el corazón de Porto</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/andorra</t>
+          <t>https://www.alojamiento.io/property/quarto-duplo-com-casa-de-banho-exclusiva-no-porto/BC-10599206</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -2791,14 +2791,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/greece</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -2816,14 +2816,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/near-me?all=true</t>
+          <t>https://www.alojamiento.io/property/fred-s-house-asprela/BC-4649516</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -2841,14 +2841,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/hotels</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=0-placeholder1&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -2866,14 +2866,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2134335&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=2-BC-2134335&amp;published=true&amp;dest_id=2134335&amp;hero=BC-1935047&amp;owner_id=2134335&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-09-04T08%3A44%3A02.076302%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/andalusia/malaga</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -2891,14 +2891,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/argentina/mendoza</t>
+          <t>https://www.alojamiento.io/all/honduras/bay-islands/roatan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -2916,14 +2916,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/romantic-luxury-house-w-captivating-outdoor-patio/BC-10659330</t>
+          <t>https://www.alojamiento.io/property/portogali-guesthouse/BC-5813166</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -2941,14 +2941,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/honduras/bay-islands/roatan</t>
+          <t>https://www.alojamiento.io/refine?search=Paranhos%2c%20Porto%2c%20Porto%20District%2c%20Portugal</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2957,7 +2957,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -2966,14 +2966,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/about-us</t>
+          <t>https://www.alojamiento.io/all/spain/community-of-madrid/madrid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -2991,14 +2991,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/catalonia/costa-brava</t>
+          <t>https://www.alojamiento.io/all/usa/wyoming/basin</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3007,7 +3007,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -3016,14 +3016,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166825172&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=9-HA-6166825172&amp;published=true&amp;dest_id=18971561&amp;hero=BC-1935047&amp;owner_id=18971561&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A03%3A04.951386%2B00%3A00</t>
+          <t>https://www.alojamiento.io/privacy-policy</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3032,7 +3032,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -3041,14 +3041,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/quintana-roo/cancun</t>
+          <t>https://www.alojamiento.io/all/spain/navarre</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -3066,14 +3066,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/community-of-madrid/madrid</t>
+          <t>https://www.alojamiento.io/all/france</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -3091,14 +3091,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/catalonia</t>
+          <t>https://www.alojamiento.io/all/mexico/guanajuato/san-miguel-de-allende</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3107,7 +3107,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -3116,14 +3116,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/italy</t>
+          <t>https://www.alojamiento.io/property/ac-house/BC-2807903</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -3141,14 +3141,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/site-map</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-1935047&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=0-BC-1935047&amp;published=true&amp;dest_id=1935047&amp;hero=BC-1935047&amp;owner_id=1935047&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-11-19T06%3A10%3A57.061047%2B00%3A00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -3166,14 +3166,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=4-placeholder5&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.onedegreeleft.com/</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -3191,14 +3191,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/cozy-apartment-invicta-city-opo/BC-11534173</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11534173&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=10-BC-11534173&amp;published=true&amp;dest_id=11534173&amp;hero=BC-1935047&amp;owner_id=11534173&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-05-12T13%3A17%3A41.359928%2B00%3A00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -3216,14 +3216,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/panama/panama/panama-city</t>
+          <t>https://www.alojamiento.io/property/jm-alojamento-local-no-porto/BC-11242224</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -3241,14 +3241,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/privacy-policy#site-cookie-policy</t>
+          <t>https://www.alojamiento.io/all/colombia/bolivar/cartagena</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3257,7 +3257,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -3266,14 +3266,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/guatemala/sacatepequez/antigua-guatemala</t>
+          <t>https://www.alojamiento.io/property/urban-views-petfrien-ap-inspired-by-torre-cl%c3%a9rigos/HA-61611682438</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -3291,14 +3291,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/place-to-stay</t>
+          <t>https://www.alojamiento.io/property/renovado-com-ac-2-wc-completos-terra%c3%a7o-e-garagem/BC-12500411</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3307,7 +3307,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -3316,14 +3316,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/urban-views-bright-apt-inspired-by-pal%c3%a1cio-cristal/HA-61611682440</t>
+          <t>https://www.alojamiento.io/property/casa-s%c3%a3o-dinis/BC-2134335</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -3341,14 +3341,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11172109&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=13-BC-11172109&amp;published=true&amp;dest_id=11172109&amp;hero=BC-1935047&amp;owner_id=11172109&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T15%3A02%3A53.704870%2B00%3A00</t>
+          <t>https://x.com/StaysTravel</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3357,7 +3357,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -3366,14 +3366,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/cuba/province-of-havana</t>
+          <t>https://www.alojamiento.io/all/puerto-rico/san-juan</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -3391,14 +3391,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/addalisting</t>
+          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-32/BC-12847446</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3407,7 +3407,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -3416,14 +3416,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11534173&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=10-BC-11534173&amp;published=true&amp;dest_id=11534173&amp;hero=BC-1935047&amp;owner_id=11534173&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-05-12T13%3A17%3A41.359928%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6118850658&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=5-HA-6118850658&amp;published=true&amp;dest_id=29545296&amp;hero=BC-1935047&amp;owner_id=29545296&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T11%3A48%3A37.454906%2B00%3A00</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -3441,14 +3441,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/argentina/buenos-aires</t>
+          <t>https://www.alojamiento.io/all/spain/valencian-community/valencia-province</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3457,7 +3457,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -3466,14 +3466,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/campo-lindo-apartment/BC-1935047</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=5-placeholder6&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -3491,14 +3491,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10998286&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=11-BC-10998286&amp;published=true&amp;dest_id=10998286&amp;hero=BC-1935047&amp;owner_id=10998286&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T07%3A15%3A38.030190%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847410&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=23-BC-12847410&amp;published=true&amp;dest_id=12847410&amp;hero=BC-1935047&amp;owner_id=12847410&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A18%3A47.203235%2B00%3A00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -3516,14 +3516,14 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10599206&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=14-BC-10599206&amp;published=true&amp;dest_id=10599206&amp;hero=BC-1935047&amp;owner_id=10599206&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-16T03%3A31%3A23.472631%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/canary-islands/gran-canaria</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -3541,14 +3541,14 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=2-placeholder3&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/spain/murcia</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3557,7 +3557,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -3566,14 +3566,14 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://x.com/StaysTravel</t>
+          <t>https://www.alojamiento.io/all/guatemala/sacatepequez/antigua-guatemala</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3598,7 +3598,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10599206&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=14-BC-10599206&amp;published=true&amp;dest_id=10599206&amp;hero=BC-1935047&amp;owner_id=10599206&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-16T03%3A31%3A23.472631%2B00%3A00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3607,7 +3607,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -3616,14 +3616,14 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/refine?search=Paranhos%2c%20Porto%2c%20Porto%20District%2c%20Portugal</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=4-placeholder5&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -3641,14 +3641,14 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/guanajuato/san-miguel-de-allende</t>
+          <t>https://www.alojamiento.io/about-us</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -3666,14 +3666,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11099494&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=17-BC-11099494&amp;published=true&amp;dest_id=11099494&amp;hero=BC-1935047&amp;owner_id=11099494&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-01T07%3A14%3A52.613135%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10998286&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=11-BC-10998286&amp;published=true&amp;dest_id=10998286&amp;hero=BC-1935047&amp;owner_id=10998286&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T07%3A15%3A38.030190%2B00%3A00</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3691,14 +3691,14 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/brazil/south-region/florianopolis</t>
+          <t>https://www.alojamiento.io/property/romantic-luxury-house-w-captivating-outdoor-patio/BC-10659330</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3707,7 +3707,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3716,14 +3716,14 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/vila-cam%c3%a9lia/BC-11099494</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cabins</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -3741,14 +3741,14 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6118850658&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=5-HA-6118850658&amp;published=true&amp;dest_id=29545296&amp;hero=BC-1935047&amp;owner_id=29545296&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T11%3A48%3A37.454906%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2134335&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=2-BC-2134335&amp;published=true&amp;dest_id=2134335&amp;hero=BC-1935047&amp;owner_id=2134335&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-09-04T08%3A44%3A02.076302%2B00%3A00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -3766,14 +3766,14 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/costa-rica/san-jose</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=2-placeholder3&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3782,7 +3782,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -3791,14 +3791,14 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11242224&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=8-BC-11242224&amp;published=true&amp;dest_id=11242224&amp;hero=BC-1935047&amp;owner_id=11242224&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T17%3A21%3A13.957523%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/belize/belize-district/belize-city</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -3816,14 +3816,14 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4649516&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=19-BC-4649516&amp;published=true&amp;dest_id=4649516&amp;hero=BC-1935047&amp;owner_id=4649516&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-08-24T10%3A49%3A52.209651%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/uruguay/montevideo</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -3841,14 +3841,14 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/modern-apartment-with-balcony-and-free-parking/BC-11172109</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11105844&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=22-BC-11105844&amp;published=true&amp;dest_id=11105844&amp;hero=BC-1935047&amp;owner_id=11105844&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T11%3A25%3A32.784787%2B00%3A00</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -3866,14 +3866,14 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/morocco</t>
+          <t>https://www.alojamiento.io/all/mexico/quintana-roo/tulum</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -3891,14 +3891,14 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/belize/belize-district/belize-city</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166491756&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=7-HA-6166491756&amp;published=true&amp;dest_id=18976742&amp;hero=BC-1935047&amp;owner_id=18976742&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A04%3A28.809814%2B00%3A00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3907,7 +3907,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3916,14 +3916,14 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/vacation-rentals</t>
+          <t>https://www.alojamiento.io/property/lux-in-porto/BC-10998286</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -3941,14 +3941,14 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.travelai.com/</t>
+          <t>https://www.instagram.com/staystravel</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3973,7 +3973,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/resorts</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2782646&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=18-BC-2782646&amp;published=true&amp;dest_id=2782646&amp;hero=BC-1935047&amp;owner_id=2782646&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-06T15%3A45%3A49.219738%2B00%3A00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3982,7 +3982,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -3991,14 +3991,14 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/colombia/medellin</t>
+          <t>https://www.alojamiento.io/all/spain/catalonia</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4007,7 +4007,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -4016,14 +4016,14 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847410&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=23-BC-12847410&amp;published=true&amp;dest_id=12847410&amp;hero=BC-1935047&amp;owner_id=12847410&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A18%3A47.203235%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/brazil/southeast-region/rio-de-janeiro</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -4041,14 +4041,14 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/poetikblue-by-we-do-living/BC-11346246</t>
+          <t>https://www.alojamiento.io/all/colombia/magdalena/santa-marta</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4057,7 +4057,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -4066,14 +4066,14 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=1-placeholder2&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/spain/catalonia/costa-brava</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4082,7 +4082,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -4091,14 +4091,14 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/baja-california-sur/cabo-san-lucas</t>
+          <t>https://www.alojamiento.io/all/chile/santiago-metropolitan/santiago</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4107,7 +4107,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -4141,14 +4141,14 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847446&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=15-BC-12847446&amp;published=true&amp;dest_id=12847446&amp;hero=BC-1935047&amp;owner_id=12847446&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A19%3A35.025518%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/ski-chalets</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4157,7 +4157,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -4166,14 +4166,14 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/s-jo%c3%a3o-porto-apartment/BC-2202420</t>
+          <t>https://www.alojamiento.io/all/cuba/province-of-havana</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4182,7 +4182,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -4191,14 +4191,14 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/navarre</t>
+          <t>https://www.alojamiento.io/property/poetikblue-by-we-do-living/BC-11346246</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4207,7 +4207,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -4216,14 +4216,14 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=5-placeholder6&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12500411&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=20-BC-12500411&amp;published=true&amp;dest_id=12500411&amp;hero=BC-1935047&amp;owner_id=12500411&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T11%3A00%3A14.620270%2B00%3A00</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4232,7 +4232,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -4241,14 +4241,14 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/castile-and-leon</t>
+          <t>https://www.alojamiento.io/faq</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4257,7 +4257,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -4266,14 +4266,14 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/jalisco/puerto-vallarta</t>
+          <t>https://www.alojamiento.io/all/mexico/baja-california-sur/cabo-san-lucas</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -4291,14 +4291,14 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/villas</t>
+          <t>https://www.alojamiento.io/all/argentina/mendoza</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4307,7 +4307,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -4316,14 +4316,14 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11105844&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=22-BC-11105844&amp;published=true&amp;dest_id=11105844&amp;hero=BC-1935047&amp;owner_id=11105844&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T11%3A25%3A32.784787%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/andorra</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -4341,14 +4341,14 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/france</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2202420&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=4-BC-2202420&amp;published=true&amp;dest_id=2202420&amp;hero=BC-1935047&amp;owner_id=2202420&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-12-06T11%3A00%3A04.420388%2B00%3A00</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -4357,7 +4357,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -4366,14 +4366,14 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/colombia/magdalena/santa-marta</t>
+          <t>https://www.alojamiento.io/property/s-jo%c3%a3o-porto-apartment/BC-2202420</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -4391,14 +4391,14 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/ac-house/BC-2807903</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cottages</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -4416,14 +4416,14 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/usa/wyoming/basin</t>
+          <t>https://www.alojamiento.io/property/lv-premier-marques-mq2-balc%c3%b3n-aire-acondicionado-vistas/HA-6118850658</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -4432,7 +4432,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -4441,14 +4441,14 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/brazil/southeast-region/rio-de-janeiro</t>
+          <t>https://www.alojamiento.io/all/mexico/jalisco/puerto-vallarta</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -4466,14 +4466,14 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/lv-premier-marques-mq2-balc%c3%b3n-aire-acondicionado-vistas/HA-6118850658</t>
+          <t>https://www.alojamiento.io/property/casa-velha-guesthouse/BC-2782646</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -4482,7 +4482,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -4491,14 +4491,14 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682438&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=3-HA-61611682438&amp;published=true&amp;dest_id=109825542&amp;hero=BC-1935047&amp;owner_id=109825542&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373667%2B00%3A00</t>
+          <t>https://www.alojamiento.io/property/t1-apartamento-moderno-luz-tranquila-y-confortable-con-garaje-privado/HA-6166491756</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -4507,7 +4507,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -4516,14 +4516,14 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/peru/cusco/cusco</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682440&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=1-HA-61611682440&amp;published=true&amp;dest_id=109825564&amp;hero=BC-1935047&amp;owner_id=109825564&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373975%2B00%3A00</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -4532,7 +4532,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -4541,14 +4541,14 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/portogali-guesthouse/BC-5813166</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/resorts</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -4566,14 +4566,14 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12500411&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=20-BC-12500411&amp;published=true&amp;dest_id=12500411&amp;hero=BC-1935047&amp;owner_id=12500411&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T11%3A00%3A14.620270%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/spain/canary-islands/tenerife</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -4591,14 +4591,14 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://www.instagram.com/staystravel</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11242224&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=8-BC-11242224&amp;published=true&amp;dest_id=11242224&amp;hero=BC-1935047&amp;owner_id=11242224&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T17%3A21%3A13.957523%2B00%3A00</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -4623,7 +4623,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/site-terms</t>
+          <t>https://www.alojamiento.io/property/campo-lindo-apartment/BC-1935047</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -4641,14 +4641,14 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/chile/santiago-metropolitan/santiago</t>
+          <t>https://www.alojamiento.io/all/spain/andalusia</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -4657,7 +4657,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -4666,14 +4666,14 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal</t>
+          <t>https://www.petfriendly.io/</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -4682,7 +4682,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -4691,14 +4691,14 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/bolivia/la-paz</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12847446&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=15-BC-12847446&amp;published=true&amp;dest_id=12847446&amp;hero=BC-1935047&amp;owner_id=12847446&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-02T08%3A19%3A35.025518%2B00%3A00</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -4707,7 +4707,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -4716,14 +4716,14 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/ecuador/pichincha/quito</t>
+          <t>https://www.alojamiento.io/site-map</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -4741,14 +4741,14 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166491756&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=7-HA-6166491756&amp;published=true&amp;dest_id=18976742&amp;hero=BC-1935047&amp;owner_id=18976742&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A04%3A28.809814%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/mexico/quintana-roo/cancun</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -4757,7 +4757,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -4766,14 +4766,14 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cottages</t>
+          <t>https://www.alojamiento.io/all/bolivia/la-paz</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -4791,14 +4791,14 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/andalusia</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11099494&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=17-BC-11099494&amp;published=true&amp;dest_id=11099494&amp;hero=BC-1935047&amp;owner_id=11099494&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-01T07%3A14%3A52.613135%2B00%3A00</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -4807,7 +4807,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -4816,14 +4816,14 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/cabins</t>
+          <t>https://www.alojamiento.io/all/peru/cusco/cusco</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -4832,7 +4832,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -4841,14 +4841,14 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/villas</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -4857,7 +4857,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -4866,14 +4866,14 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/rendez-vous-porto-ii-t1/HA-6166825172</t>
+          <t>https://www.alojamiento.io/property/modern-apartment-with-balcony-and-free-parking/BC-11172109</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4882,7 +4882,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -4891,14 +4891,14 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/jm-alojamento-local-no-porto/BC-11242224</t>
+          <t>https://www.alojamiento.io/all/portugal</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -4916,14 +4916,14 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/argentina/rio-negro/san-carlos-de-bariloche</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=1-placeholder2&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -4941,14 +4941,14 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/valencian-community/valencia-province</t>
+          <t>https://www.alojamiento.io/all/costa-rica/san-jose</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -4957,7 +4957,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -4966,14 +4966,14 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/ecuador/galapagos</t>
+          <t>https://www.alojamiento.io/all/spain/castile-and-leon</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -4991,14 +4991,14 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.onedegreeleft.com/</t>
+          <t>https://www.alojamiento.io/all/spain/balearic-islands</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -5023,7 +5023,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682440&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=1-HA-61611682440&amp;published=true&amp;dest_id=109825564&amp;hero=BC-1935047&amp;owner_id=109825564&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373975%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/greece</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -5032,7 +5032,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -5041,14 +5041,14 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/peru/lima</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4649516&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=19-BC-4649516&amp;published=true&amp;dest_id=4649516&amp;hero=BC-1935047&amp;owner_id=4649516&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-08-24T10%3A49%3A52.209651%2B00%3A00</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -5057,7 +5057,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -5066,14 +5066,14 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=0-placeholder1&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/all/switzerland</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -5091,14 +5091,14 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/StaysTravel</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10659330&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=12-BC-10659330&amp;published=true&amp;dest_id=10659330&amp;hero=BC-1935047&amp;owner_id=10659330&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T06%3A05%3A00.026562%2B00%3A00</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -5123,7 +5123,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/faq</t>
+          <t>https://www.alojamiento.io/site-terms</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -5132,7 +5132,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -5141,14 +5141,14 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-31/BC-12847410</t>
+          <t>https://www.alojamiento.io/</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -5157,7 +5157,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -5166,14 +5166,14 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/switzerland</t>
+          <t>https://www.travelai.com/</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -5191,14 +5191,14 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/quarto-duplo-com-casa-de-banho-exclusiva-no-porto/BC-10599206</t>
+          <t>https://www.alojamiento.io/all/spain/galicia</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -5207,7 +5207,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -5216,14 +5216,14 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/murcia</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2807903&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=16-BC-2807903&amp;published=true&amp;dest_id=2807903&amp;hero=BC-1935047&amp;owner_id=2807903&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-11-19T09%3A57%3A24.866726%2B00%3A00</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -5232,7 +5232,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -5241,14 +5241,14 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/t1-apartamento-moderno-luz-tranquila-y-confortable-con-garaje-privado/HA-6166491756</t>
+          <t>https://www.alojamiento.io/property/cozy-apartment-invicta-city-opo/BC-11534173</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -5257,7 +5257,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -5266,14 +5266,14 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/dominican-republic/la-altagracia/punta-cana</t>
+          <t>https://www.alojamiento.io/place-to-stay</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -5282,7 +5282,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -5291,14 +5291,14 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.petfriendly.io/</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5813166&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=6-BC-5813166&amp;published=true&amp;dest_id=5813166&amp;hero=BC-1935047&amp;owner_id=5813166&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-08-16T12%3A45%3A47.750380%2B00%3A00</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -5307,7 +5307,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -5316,14 +5316,14 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos</t>
+          <t>https://www.alojamiento.io/property/vila-cam%c3%a9lia/BC-11099494</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -5332,7 +5332,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -5341,14 +5341,14 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/balearic-islands</t>
+          <t>https://www.alojamiento.io/all/brazil/south-region/florianopolis</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -5357,7 +5357,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -5366,14 +5366,14 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/cantabria</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/vacation-rentals</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -5382,7 +5382,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -5391,14 +5391,14 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10659330&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=12-BC-10659330&amp;published=true&amp;dest_id=10659330&amp;hero=BC-1935047&amp;owner_id=10659330&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-04T06%3A05%3A00.026562%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -5407,7 +5407,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -5416,14 +5416,14 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/casa-s%c3%a3o-dinis/BC-2134335</t>
+          <t>https://www.alojamiento.io/all/argentina/buenos-aires</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -5441,14 +5441,14 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11346246&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=21-BC-11346246&amp;published=true&amp;dest_id=11346246&amp;hero=BC-1935047&amp;owner_id=11346246&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-09-22T08%3A32%3A12.548999%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/mexico/quintana-roo/playa-del-carmen</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -5457,7 +5457,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -5466,14 +5466,14 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-1935047&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=0-BC-1935047&amp;published=true&amp;dest_id=1935047&amp;hero=BC-1935047&amp;owner_id=1935047&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-11-19T06%3A10%3A57.061047%2B00%3A00</t>
+          <t>https://www.alojamiento.io/near-me?all=true</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -5482,7 +5482,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -5491,14 +5491,14 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/galicia</t>
+          <t>https://www.alojamiento.io/privacy-policy#site-cookie-policy</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -5507,7 +5507,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -5516,14 +5516,14 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-32/BC-12847446</t>
+          <t>https://www.alojamiento.io/property/urban-views-bright-apt-inspired-by-pal%c3%a1cio-cristal/HA-61611682440</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -5532,7 +5532,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -5541,14 +5541,14 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2782646&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=18-BC-2782646&amp;published=true&amp;dest_id=2782646&amp;hero=BC-1935047&amp;owner_id=2782646&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-07-06T15%3A45%3A49.219738%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -5557,7 +5557,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -5566,14 +5566,14 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/colombia/bolivar/cartagena</t>
+          <t>https://www.alojamiento.io/all/panama/panama/panama-city</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -5582,7 +5582,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -5591,14 +5591,14 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=3-placeholder4&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6166825172&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=9-HA-6166825172&amp;published=true&amp;dest_id=18971561&amp;hero=BC-1935047&amp;owner_id=18971561&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c999&amp;upat=2024-12-04T10%3A03%3A04.951386%2B00%3A00</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -5616,14 +5616,14 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/canary-islands/gran-canaria</t>
+          <t>https://www.alojamiento.io/all/colombia/medellin</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -5632,7 +5632,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -5641,14 +5641,14 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/fred-s-house-asprela/BC-4649516</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11346246&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=21-BC-11346246&amp;published=true&amp;dest_id=11346246&amp;hero=BC-1935047&amp;owner_id=11346246&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-09-22T08%3A32%3A12.548999%2B00%3A00</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -5657,7 +5657,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -5666,14 +5666,14 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/ski-chalets</t>
+          <t>https://www.alojamiento.io/property/the-cale-antero-de-quental-31/BC-12847410</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -5682,7 +5682,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -5691,14 +5691,14 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/privacy-policy</t>
+          <t>https://www.alojamiento.io/all/spain/cantabria</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -5707,7 +5707,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -5716,14 +5716,14 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/portugal/porto-district</t>
+          <t>https://www.facebook.com/StaysTravel</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -5731,24 +5731,21 @@
           <t>URL Status Code Test</t>
         </is>
       </c>
-      <c r="C120" t="n">
-        <v>403</v>
-      </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>passed</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x7eca4d324bc0&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/lovely-flat-marqu%c3%aas/BC-11105844</t>
+          <t>https://www.alojamiento.io/all/ecuador/pichincha/quito</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -5757,7 +5754,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -5766,14 +5763,14 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/uruguay/montevideo</t>
+          <t>https://www.alojamiento.io/all/ecuador/galapagos</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -5782,7 +5779,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -5791,14 +5788,14 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/brazil/northeast-region/salvador</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-61611682438&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=3-HA-61611682438&amp;published=true&amp;dest_id=109825542&amp;hero=BC-1935047&amp;owner_id=109825542&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;epc=c001&amp;upat=2024-12-05T01%3A44%3A21.373667%2B00%3A00</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -5807,7 +5804,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -5816,14 +5813,14 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/quintana-roo/tulum</t>
+          <t>https://www.alojamiento.io/all/peru/lima</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -5832,7 +5829,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -5841,14 +5838,14 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/canary-islands/tenerife</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11172109&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=13-BC-11172109&amp;published=true&amp;dest_id=11172109&amp;hero=BC-1935047&amp;owner_id=11172109&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-12-05T15%3A02%3A53.704870%2B00%3A00</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -5857,7 +5854,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -5866,14 +5863,14 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/mexico/quintana-roo/playa-del-carmen</t>
+          <t>https://www.alojamiento.io/property/rendez-vous-porto-ii-t1/HA-6166825172</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -5882,7 +5879,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -5891,14 +5888,14 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/urban-views-petfrien-ap-inspired-by-torre-cl%c3%a9rigos/HA-61611682438</t>
+          <t>https://www.alojamiento.io/all/italy</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -5907,7 +5904,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -5916,14 +5913,14 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5813166&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=6-BC-5813166&amp;published=true&amp;dest_id=5813166&amp;hero=BC-1935047&amp;owner_id=5813166&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-08-16T12%3A45%3A47.750380%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Paranhos,%20Porto,%20Porto%20District,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733892318747&amp;referral_id=3-placeholder4&amp;hero=BC-1935047&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -5932,7 +5929,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -5941,14 +5938,14 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/casa-velha-guesthouse/BC-2782646</t>
+          <t>https://www.alojamiento.io/all/portugal/porto-district/porto/paranhos/hotels</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -5957,7 +5954,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -5966,14 +5963,14 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2202420&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=4-BC-2202420&amp;published=true&amp;dest_id=2202420&amp;hero=BC-1935047&amp;owner_id=2202420&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2023-12-06T11%3A00%3A04.420388%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/dominican-republic/la-altagracia/punta-cana</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -5982,7 +5979,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
@@ -5991,14 +5988,14 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/puerto-rico/san-juan</t>
+          <t>https://www.alojamiento.io/all/mexico</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -6007,7 +6004,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -6016,14 +6013,14 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-2807903&amp;guests=2&amp;search_string=Porto,%20Portugal&amp;referrer_page=hybrid&amp;menu_id=1733847445262&amp;referral_id=16-BC-2807903&amp;published=true&amp;dest_id=2807903&amp;hero=BC-1935047&amp;owner_id=2807903&amp;sqs=hybrid-default&amp;property_country=PT&amp;at=End-of-Result%20Ad&amp;eplId=6336340&amp;upat=2024-11-19T09%3A57%3A24.866726%2B00%3A00</t>
+          <t>https://www.alojamiento.io/all/brazil/northeast-region/salvador</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -6032,7 +6029,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -6041,14 +6038,14 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/all/spain/andalusia/malaga</t>
+          <t>https://www.alojamiento.io/addalisting</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -6057,7 +6054,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -6066,14 +6063,14 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/lux-in-porto/BC-10998286</t>
+          <t>https://www.alojamiento.io/all/argentina/rio-negro/san-carlos-de-bariloche</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -6082,7 +6079,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -6091,14 +6088,14 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/property/renovado-com-ac-2-wc-completos-terra%c3%a7o-e-garagem/BC-12500411</t>
+          <t>https://www.alojamiento.io/property/lovely-flat-marqu%c3%aas/BC-11105844</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -6107,7 +6104,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -6116,14 +6113,14 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/all/morocco</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -6132,7 +6129,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>403</v>
+        <v>200</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -6141,7 +6138,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Status code 403 (Forbidden)</t>
+          <t>Status code 200 (OK)</t>
         </is>
       </c>
     </row>
@@ -6156,7 +6153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10225,6 +10222,1350 @@
         </is>
       </c>
       <c r="F145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>1</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>De €102</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>De د.إ.395</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>2</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>De €118</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>De د.إ.460</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>3</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>De €181</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>De د.إ.705</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>4</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>De €111</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>De د.إ.431</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>5</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>De €40</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>De د.إ.155</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>6</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>De €185</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>De د.إ.720</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>7</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>De €48</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>De د.إ.185</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>8</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>De €54</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>De د.إ.210</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>9</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>De €146</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>De د.إ.566</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>10</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>De €68</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>De د.إ.264</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>11</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>De €92</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>De د.إ.356</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>12</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>De €94</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>De د.إ.364</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>13</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>De €98</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>De د.إ.382</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>14</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>De €83</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>De د.إ.323</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>15</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>De €63</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>De د.إ.246</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>16</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>De €105</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>De د.إ.409</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>17</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>De €30</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>De د.إ.117</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>18</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>De €104</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>De د.إ.404</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>19</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>De €72</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>De د.إ.279</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>20</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>De €78</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>De د.إ.302</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>21</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>De €142</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>De د.إ.551</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>22</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>De €71</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>De د.إ.277</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F167" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>23</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>De €184</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>De د.إ.716</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F168" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>د.إ.‏ (AED)</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>24</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>De €105</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>De د.إ.409</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>AED د.إ.395</t>
+        </is>
+      </c>
+      <c r="F169" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>1</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>De €102</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>De ৳12,890</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F170" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>2</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>De €118</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>De ৳15,027</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F171" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>3</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>De €181</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>De ৳23,021</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F172" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>4</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>De €111</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>De ৳14,078</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F173" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>5</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>De €40</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>De ৳5,067</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F174" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>6</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>De €185</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>De ৳23,514</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F175" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>7</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>De €48</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>De ৳6,043</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F176" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>8</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>De €54</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>De ৳6,848</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F177" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>9</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>De €146</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>De ৳18,465</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F178" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>10</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>De €68</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>De ৳8,623</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F179" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>11</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>De €92</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>De ৳11,631</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F180" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>12</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>De €94</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>De ৳11,870</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F181" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>13</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>De €98</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>De ৳12,470</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F182" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>14</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>De €83</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>De ৳10,551</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F183" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>15</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>De €63</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>De ৳8,034</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F184" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>16</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>De €105</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>De ৳13,348</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F185" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>17</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>De €30</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>De ৳3,807</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F186" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>18</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>De €104</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>De ৳13,189</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F187" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>19</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>De €72</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>De ৳9,113</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F188" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>20</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>De €78</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>De ৳9,869</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F189" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>21</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>De €142</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>De ৳17,985</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F190" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>22</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>De €71</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>De ৳9,047</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F191" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>23</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>De €184</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>De ৳23,381</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>৳ (BDT)</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>24</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>De €105</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>De ৳13,348</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>BDT ৳12,890</t>
+        </is>
+      </c>
+      <c r="F193" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10307,7 +11648,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>103.149.143.25</t>
+          <t>182.160.106.203</t>
         </is>
       </c>
     </row>

</xml_diff>